<commit_message>
docs (presentation): Create ppt file to present the project
</commit_message>
<xml_diff>
--- a/conception/dictionnaireDesDonnees_v2.xlsx
+++ b/conception/dictionnaireDesDonnees_v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v.masson\Documents\Projets de Stage\SGPC\conception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projets de Stage\SGPC\conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="179">
   <si>
     <t>Code</t>
   </si>
@@ -119,9 +119,6 @@
     <t>nom</t>
   </si>
   <si>
-    <t>prénom</t>
-  </si>
-  <si>
     <t>e-mail</t>
   </si>
   <si>
@@ -131,24 +128,12 @@
     <t>date de fin de droit</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
     <t>mail</t>
   </si>
   <si>
     <t>endRightDate</t>
   </si>
   <si>
-    <t>Nom de l'utilisateur</t>
-  </si>
-  <si>
-    <t>Prénom de l'utilisateur</t>
-  </si>
-  <si>
     <t>Email de l'utilisateur</t>
   </si>
   <si>
@@ -555,6 +540,33 @@
   </si>
   <si>
     <t>Phrase de conseil de prudence</t>
+  </si>
+  <si>
+    <t>nom et prénom</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>Nom et prénom de l'utilisateur</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Login de connexion de l'utilisateur</t>
+  </si>
+  <si>
+    <t>fiche de risque</t>
+  </si>
+  <si>
+    <t>Fiche de risque du produit</t>
+  </si>
+  <si>
+    <t>dangerFile</t>
   </si>
 </sst>
 </file>
@@ -1239,10 +1251,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1326,13 +1338,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>170</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>172</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>7</v>
@@ -1344,43 +1356,47 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>29</v>
+        <v>173</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>38</v>
+        <v>175</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>15</v>
@@ -1392,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1400,13 +1416,13 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>12</v>
@@ -1429,7 +1445,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
@@ -1444,10 +1460,10 @@
         <v>24</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>20</v>
@@ -1464,10 +1480,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>11</v>
@@ -1481,13 +1497,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>7</v>
@@ -1499,13 +1515,13 @@
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>8</v>
@@ -1528,7 +1544,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -1543,10 +1559,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>20</v>
@@ -1563,10 +1579,10 @@
         <v>28</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>11</v>
@@ -1580,7 +1596,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -1595,10 +1611,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>20</v>
@@ -1612,13 +1628,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>11</v>
@@ -1632,7 +1648,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
@@ -1647,10 +1663,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>20</v>
@@ -1667,10 +1683,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>7</v>
@@ -1684,13 +1700,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>7</v>
@@ -1704,13 +1720,13 @@
     </row>
     <row r="29" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>11</v>
@@ -1724,16 +1740,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
@@ -1744,13 +1760,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>21</v>
@@ -1772,7 +1788,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -1787,10 +1803,10 @@
         <v>24</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>20</v>
@@ -1804,13 +1820,13 @@
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>12</v>
@@ -1822,63 +1838,63 @@
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G36" s="23"/>
       <c r="H36" s="23"/>
     </row>
     <row r="37" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -1886,13 +1902,13 @@
     </row>
     <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>11</v>
@@ -1908,20 +1924,20 @@
     </row>
     <row r="40" spans="1:8" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6" t="s">
@@ -1930,13 +1946,13 @@
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>12</v>
@@ -1948,632 +1964,650 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D42" s="9" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="7"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="5"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="33"/>
+    </row>
+    <row r="46" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="33"/>
-    </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="D47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="G48" s="22"/>
+      <c r="H48" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="29"/>
+    </row>
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22" t="s">
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="29"/>
+    </row>
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="29"/>
-    </row>
-    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="C56" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="29"/>
+    </row>
+    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" s="11" t="s">
+      <c r="B59" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E59" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="9" t="s">
+      <c r="B60" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+    </row>
+    <row r="62" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="26"/>
+    </row>
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="25"/>
+      <c r="H66" s="26"/>
+    </row>
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="28"/>
+      <c r="H70" s="29"/>
+    </row>
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="29"/>
-    </row>
-    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="35"/>
+      <c r="H75" s="36"/>
+    </row>
+    <row r="76" spans="1:8" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="11" t="s">
+      <c r="B76" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D76" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E76" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="4"/>
+    </row>
+    <row r="77" spans="1:8" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="9" t="s">
+      <c r="B78" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="29"/>
-    </row>
-    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="10"/>
+    </row>
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="26"/>
+    </row>
+    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="B81" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D81" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E81" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E59" s="9" t="s">
+      <c r="B83" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-    </row>
-    <row r="61" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="26"/>
-    </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="26"/>
-    </row>
-    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="29"/>
-    </row>
-    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="35"/>
-      <c r="H74" s="36"/>
-    </row>
-    <row r="75" spans="1:8" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C75" s="11" t="s">
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="18"/>
+      <c r="C86" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D75" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="10"/>
-    </row>
-    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="26"/>
-    </row>
-    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" s="4"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="18"/>
-      <c r="C85" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="5"/>
-      <c r="C86" s="7"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="19"/>
-      <c r="C87" s="10" t="s">
+      <c r="B87" s="5"/>
+      <c r="C87" s="7"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="19"/>
+      <c r="C88" s="10" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A57:H57"/>
-    <mergeCell ref="A69:H69"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="A70:H70"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A61:H61"/>
-    <mergeCell ref="A65:H65"/>
-    <mergeCell ref="A74:H74"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A75:H75"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A50:H50"/>
     <mergeCell ref="A33:H33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>